<commit_message>
Busqueda de datos en el PJUD  iniciada y en proceso
</commit_message>
<xml_diff>
--- a/Controller/Remates.xlsx
+++ b/Controller/Remates.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B5:S24"/>
+  <dimension ref="B5:S37"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -954,9 +954,347 @@
         <v>Mínimo subasta 4963,3864 U.F.</v>
       </c>
     </row>
+    <row r="24">
+      <c r="B24" t="str">
+        <v>https://www.economicos.cl/remates/clasificados-remates-cod47442289.html</v>
+      </c>
+      <c r="C24" s="1">
+        <v>45636.99947916667</v>
+      </c>
+      <c r="D24" s="1">
+        <v>45545.99947916667</v>
+      </c>
+      <c r="F24" t="str">
+        <v>C-10640-2023</v>
+      </c>
+      <c r="G24" t="str">
+        <v>3° juzgado civil de santiago</v>
+      </c>
+      <c r="P24" t="str">
+        <v>vale vista</v>
+      </c>
+      <c r="Q24" t="str">
+        <v>10% del mínimo</v>
+      </c>
+      <c r="S24" t="str">
+        <v>Mínimo para iniciar posturas $ 49.736.202</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="str">
+        <v>https://www.economicos.cl/remates/clasificados-remates-cod7478522.html</v>
+      </c>
+      <c r="C25" s="1">
+        <v>45636.99947916667</v>
+      </c>
+      <c r="D25" s="1">
+        <v>45545.99947916667</v>
+      </c>
+      <c r="F25" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="G25" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="P25" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="Q25" t="str">
+        <v>Garantía 10%</v>
+      </c>
+      <c r="S25" t="str">
+        <v>Mínimo $ 37.506.795</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="str">
+        <v>https://www.economicos.cl/remates/clasificados-remates-cod47442024.html</v>
+      </c>
+      <c r="C26" s="1">
+        <v>45636.99947916667</v>
+      </c>
+      <c r="D26" s="1">
+        <v>45545.99947916667</v>
+      </c>
+      <c r="F26" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="G26" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="P26" t="str">
+        <v>vale vista</v>
+      </c>
+      <c r="Q26" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="S26" t="str">
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="str">
+        <v>https://www.economicos.cl/remates/clasificados-remates-cod47444967.html</v>
+      </c>
+      <c r="C27" s="1">
+        <v>45636.99947916667</v>
+      </c>
+      <c r="D27" s="1">
+        <v>45545.99947916667</v>
+      </c>
+      <c r="F27" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="G27" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="P27" t="str">
+        <v>vale vista</v>
+      </c>
+      <c r="Q27" t="str">
+        <v>Garantía 10%</v>
+      </c>
+      <c r="S27" t="str">
+        <v>Mínimo $40.000.000</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="str">
+        <v>https://www.economicos.cl/remates/clasificados-remates-cod47463302.html</v>
+      </c>
+      <c r="C28" s="1">
+        <v>45636.99947916667</v>
+      </c>
+      <c r="D28" s="1">
+        <v>45545.99947916667</v>
+      </c>
+      <c r="F28" t="str">
+        <v>c-1275-2023</v>
+      </c>
+      <c r="G28" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="P28" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="Q28" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="S28" t="str">
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="str">
+        <v>https://www.economicos.cl/remates/clasificados-remates-cod7478514.html</v>
+      </c>
+      <c r="C29" s="1">
+        <v>45636.99947916667</v>
+      </c>
+      <c r="D29" s="1">
+        <v>45545.99947916667</v>
+      </c>
+      <c r="F29" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="G29" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="P29" t="str">
+        <v>Vale Vista</v>
+      </c>
+      <c r="Q29" t="str">
+        <v>caución de un 10%</v>
+      </c>
+      <c r="S29" t="str">
+        <v>Mínimo para la subasta es la suma de $ 138.000.000</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="str">
+        <v>https://www.economicos.cl/remates/clasificados-remates-cod7478519.html</v>
+      </c>
+      <c r="C30" s="1">
+        <v>45636.99947916667</v>
+      </c>
+      <c r="D30" s="1">
+        <v>45545.99947916667</v>
+      </c>
+      <c r="F30" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="G30" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="P30" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="Q30" t="str">
+        <v>Garantía 10%</v>
+      </c>
+      <c r="S30" t="str">
+        <v>Mínimo $ 80.000.000</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="str">
+        <v>https://www.economicos.cl/remates/clasificados-remates-cod47419724.html</v>
+      </c>
+      <c r="C31" s="1">
+        <v>45636.99947916667</v>
+      </c>
+      <c r="D31" s="1">
+        <v>45545.99947916667</v>
+      </c>
+      <c r="F31" t="str">
+        <v>C-3627-2023</v>
+      </c>
+      <c r="G31" t="str">
+        <v>1° juzgado de letras de melipilla</v>
+      </c>
+      <c r="P31" t="str">
+        <v>vale vista</v>
+      </c>
+      <c r="Q31" t="str">
+        <v>10% del mínimo</v>
+      </c>
+      <c r="S31" t="str">
+        <v>mínimo postura: $ 244.000.000</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="str">
+        <v>https://www.economicos.cl/remates/clasificados-remates-cod47445130.html</v>
+      </c>
+      <c r="C32" s="1">
+        <v>45636.99947916667</v>
+      </c>
+      <c r="D32" s="1">
+        <v>45545.99947916667</v>
+      </c>
+      <c r="F32" t="str">
+        <v>C-4117-2024</v>
+      </c>
+      <c r="G32" t="str">
+        <v>2° juzgado civil de santiago</v>
+      </c>
+      <c r="P32" t="str">
+        <v>vale vista</v>
+      </c>
+      <c r="Q32" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="S32" t="str">
+        <v>mínimo para la subasta será la suma de $ 250.838.785</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="str">
+        <v>https://www.economicos.cl/remates/clasificados-remates-cod7477212.html</v>
+      </c>
+      <c r="C33" s="1">
+        <v>45636.99947916667</v>
+      </c>
+      <c r="D33" s="1">
+        <v>45545.99947916667</v>
+      </c>
+      <c r="F33" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="G33" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="P33" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="Q33" t="str">
+        <v>Garantía 10%</v>
+      </c>
+      <c r="S33" t="str">
+        <v>Mínimo $ 45.000.000</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="str">
+        <v>https://www.economicos.cl/remates/clasificados-remates-cod47442147.html</v>
+      </c>
+      <c r="C34" s="1">
+        <v>45636.99947916667</v>
+      </c>
+      <c r="D34" s="1">
+        <v>45545.99947916667</v>
+      </c>
+      <c r="F34" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="G34" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="P34" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="Q34" t="str">
+        <v>Garantía 10%</v>
+      </c>
+      <c r="S34" t="str">
+        <v>Mínimo UF 3.567</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="str">
+        <v>https://www.economicos.cl/remates/clasificados-remates-cod47445033.html</v>
+      </c>
+      <c r="C35" s="1">
+        <v>45636.99947916667</v>
+      </c>
+      <c r="D35" s="1">
+        <v>45545.99947916667</v>
+      </c>
+      <c r="F35" t="str">
+        <v>C-26213-2019</v>
+      </c>
+      <c r="G35" t="str">
+        <v>6° juzgado civil de santiago</v>
+      </c>
+      <c r="P35" t="str">
+        <v>vale vista</v>
+      </c>
+      <c r="Q35" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="S35" t="str">
+        <v>mínimo para iniciar las posturas: $ 91.901.468</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="str">
+        <v>https://www.economicos.cl/remates/clasificados-remates-cod47458046.html</v>
+      </c>
+      <c r="C36" s="1">
+        <v>45636.99947916667</v>
+      </c>
+      <c r="D36" s="1">
+        <v>45545.99947916667</v>
+      </c>
+      <c r="F36" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="G36" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="P36" t="str">
+        <v>vale vista</v>
+      </c>
+      <c r="Q36" t="str">
+        <v>interesados equivalente al 10%</v>
+      </c>
+      <c r="S36" t="str">
+        <v>Mínimo: $70.308.933</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="B5:S24"/>
+    <ignoredError numberStoredAsText="1" sqref="B5:S37"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>